<commit_message>
I am investigating alternative quarter schemes. Next is 4-4-5.
</commit_message>
<xml_diff>
--- a/QuarterDetermination.xlsx
+++ b/QuarterDetermination.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{F11932D1-4811-44CE-8735-4BCA25183E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5426E4B-E441-4F68-B029-C426F2089D8B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8980CD1-30F9-4C8F-B087-5FDB457C8D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36360" yWindow="1815" windowWidth="20130" windowHeight="15555" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>FROM:</t>
   </si>
@@ -184,6 +186,12 @@
   </si>
   <si>
     <t>Every work week starts on Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grant has heard of the 4-5-4 but never used it. </t>
+  </si>
+  <si>
+    <t>I see there is also a 4-4-5 approach. Makes sense. Only has to sum to 13 weeks.</t>
   </si>
 </sst>
 </file>
@@ -421,7 +429,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -434,7 +442,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9"/>
@@ -868,7 +875,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1171,10 +1178,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1203,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>27</v>
       </c>
       <c r="J1" t="s">
@@ -1216,7 +1223,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="J2" s="14">
+      <c r="J2" s="13">
         <v>45166</v>
       </c>
       <c r="K2">
@@ -1236,12 +1243,12 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>01-Feb-2024</v>
+        <v>03-Feb-2024</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <v>45194</v>
       </c>
       <c r="K3">
@@ -1253,7 +1260,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>45222</v>
       </c>
       <c r="K4">
@@ -1265,7 +1272,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>45257</v>
       </c>
       <c r="K5">
@@ -1289,7 +1296,7 @@
       <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>45285</v>
       </c>
       <c r="K6">
@@ -1301,7 +1308,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>45310</v>
       </c>
       <c r="B7" t="str">
@@ -1316,7 +1323,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A7,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>2</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <v>45313</v>
       </c>
       <c r="K7">
@@ -1328,7 +1335,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>45347</v>
       </c>
       <c r="B8" t="str">
@@ -1343,7 +1350,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A8,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>2</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <v>45348</v>
       </c>
       <c r="K8">
@@ -1355,7 +1362,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>45406</v>
       </c>
       <c r="B9" t="str">
@@ -1370,7 +1377,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A9,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>3</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <v>45376</v>
       </c>
       <c r="K9">
@@ -1382,7 +1389,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>45467</v>
       </c>
       <c r="B10" t="str">
@@ -1397,7 +1404,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A10,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>4</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <v>45404</v>
       </c>
       <c r="K10">
@@ -1409,7 +1416,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>45552</v>
       </c>
       <c r="B11" t="str">
@@ -1424,7 +1431,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A11,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>1</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <v>45439</v>
       </c>
       <c r="K11">
@@ -1436,7 +1443,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>45587</v>
       </c>
       <c r="B12" t="str">
@@ -1451,7 +1458,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A12,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>1</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <v>45467</v>
       </c>
       <c r="K12">
@@ -1463,7 +1470,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>45622</v>
       </c>
       <c r="B13" t="str">
@@ -1478,7 +1485,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A13,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>2</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="13">
         <v>45495</v>
       </c>
       <c r="K13">
@@ -1490,7 +1497,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>45631</v>
       </c>
       <c r="B14" t="str">
@@ -1505,7 +1512,7 @@
         <f>ROUNDUP(_xlfn.XLOOKUP(A14,Table2[Period Start Date],Table2[Period],"Not Found",-1)/3,0)</f>
         <v>2</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <v>45530</v>
       </c>
       <c r="K14">
@@ -1517,7 +1524,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <v>45558</v>
       </c>
       <c r="K15">
@@ -1529,10 +1536,10 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <v>45586</v>
       </c>
       <c r="K16">
@@ -1547,7 +1554,7 @@
       <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <v>45621</v>
       </c>
       <c r="K17">
@@ -1562,7 +1569,7 @@
       <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <v>45649</v>
       </c>
       <c r="K18">
@@ -1574,13 +1581,23 @@
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1637,7 +1654,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>01-Feb-2024</v>
+        <v>03-Feb-2024</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1774,19 +1791,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1794,11 +1807,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12">
-        <v>2</v>
-      </c>
-      <c r="F21" s="12">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1806,19 +1818,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1826,11 +1834,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1838,19 +1845,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1858,11 +1861,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1870,13 +1872,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -1962,7 +1964,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>01-Feb-2024</v>
+        <v>03-Feb-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>